<commit_message>
extra code 5/7 p1 and p2
</commit_message>
<xml_diff>
--- a/src/route/excel/giaovien.xlsx
+++ b/src/route/excel/giaovien.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -40,22 +40,10 @@
     <t xml:space="preserve">nguyen thi thu </t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nguyen thi dong </t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t xml:space="preserve">nguyen thi a </t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nguyen thi b </t>
   </si>
 </sst>
 </file>
@@ -432,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,35 +469,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>